<commit_message>
SMD After BOM Update
</commit_message>
<xml_diff>
--- a/- DOCS -/COMPONENTS LIST/After_Rybnik_BOM.xlsx
+++ b/- DOCS -/COMPONENTS LIST/After_Rybnik_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\RoboCop\- PCB -\SUMEC SMD-V2\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\RoboCop\- DOCS -\COMPONENTS LIST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C58A9-DAB3-488A-8BFE-82975BA1C0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE1DA0A-3995-46F4-976D-ED54FDD94503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,20 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Designator</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>DRV8874</t>
   </si>
   <si>
@@ -59,27 +53,6 @@
     <t>SW_Push</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>MountingHole_3.2mm_M3_Pad</t>
-  </si>
-  <si>
-    <t>MountingHole_Pad</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>SolderWire-0.1sqmm_1x01_D0.4mm_OD1mm</t>
-  </si>
-  <si>
-    <t>Conn_01x01_Pin</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
     <t>TO-263-3_TabPin2</t>
   </si>
   <si>
@@ -98,9 +71,6 @@
     <t>TYPE-C-31-M-12</t>
   </si>
   <si>
-    <t>D3</t>
-  </si>
-  <si>
     <t>D_Schottky</t>
   </si>
   <si>
@@ -113,9 +83,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>LM1084-3.3</t>
   </si>
   <si>
@@ -128,24 +95,15 @@
     <t>Conn_01x06_Pin</t>
   </si>
   <si>
-    <t>U3</t>
-  </si>
-  <si>
     <t>TSOT-23-6_HandSoldering</t>
   </si>
   <si>
     <t>USBLC6-2SC6</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>ESP32-S3-WROOM-1</t>
   </si>
   <si>
-    <t>U5</t>
-  </si>
-  <si>
     <t>TSOP</t>
   </si>
   <si>
@@ -167,21 +125,12 @@
     <t>0R</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>JST_XH_B4B-XH-A_1x04_P2.50mm_Vertical</t>
-  </si>
-  <si>
     <t>Conn_01x04_Pin</t>
   </si>
   <si>
     <t>10k</t>
   </si>
   <si>
-    <t>J3</t>
-  </si>
-  <si>
     <t>Molex_PicoBlade_53398-0471_1x04-1MP_P1.25mm_Vertical</t>
   </si>
   <si>
@@ -194,9 +143,6 @@
     <t>Molex_PicoBlade_53261-0471_1x04-1MP_P1.25mm_Horizontal</t>
   </si>
   <si>
-    <t>U2,U1</t>
-  </si>
-  <si>
     <t>OnSemi_CASE100AQ - QRE1113</t>
   </si>
   <si>
@@ -281,66 +227,18 @@
     <t>SPDT Switch, mouser</t>
   </si>
   <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>J10,J8,J7</t>
-  </si>
-  <si>
-    <t>SW2</t>
-  </si>
-  <si>
     <t>XT30PW-M</t>
   </si>
   <si>
     <t>AMASS_XT30PW-M</t>
   </si>
   <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>J5,J4,J6</t>
-  </si>
-  <si>
-    <t>R7,R6</t>
-  </si>
-  <si>
     <t>D_1206_3216Metric_Pad1.42x1.75mm_HandSolder</t>
   </si>
   <si>
     <t>22nF.hb</t>
   </si>
   <si>
-    <t>C3,C4</t>
-  </si>
-  <si>
-    <t>SW1,SW4,SW3</t>
-  </si>
-  <si>
-    <t>IC1,IC2</t>
-  </si>
-  <si>
-    <t>H1,H3,H2 - H1, H2</t>
-  </si>
-  <si>
-    <t>C1,C9,C10,C15,C14,C19,C17,C18,C16</t>
-  </si>
-  <si>
-    <t>R20, R21</t>
-  </si>
-  <si>
-    <t>R2D2, Logo</t>
-  </si>
-  <si>
-    <t>C2,C13,C5,C6,C7,C8,C11,C12</t>
-  </si>
-  <si>
-    <t>R9,R8 - R4,R2</t>
-  </si>
-  <si>
     <t>22nF, 50V, 0805, ceramic, mouser, X7R</t>
   </si>
   <si>
@@ -350,24 +248,9 @@
     <t>Red LED, 20mA 1.9V, 0805, mouser</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
     <t>Yellow LED, 20mA, 1.9V, 0805, mouser</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R1,R2,R10 - R3,R1</t>
-  </si>
-  <si>
     <t>560R, 500mW, 0805, mouser</t>
   </si>
   <si>
@@ -386,13 +269,73 @@
     <t>Green-Yellow LED, 20mA, 1.9V, mouser</t>
   </si>
   <si>
-    <t>100?</t>
-  </si>
-  <si>
-    <t>50?</t>
-  </si>
-  <si>
-    <t>15 + 4 pujceno + 10 doma</t>
+    <t>100nf</t>
+  </si>
+  <si>
+    <t>esp32 s3 wroom2</t>
+  </si>
+  <si>
+    <t>usbc</t>
+  </si>
+  <si>
+    <t>ucbc</t>
+  </si>
+  <si>
+    <t>s-diode</t>
+  </si>
+  <si>
+    <t>qre smd</t>
+  </si>
+  <si>
+    <t>qresmd</t>
+  </si>
+  <si>
+    <t>esp32 s3 wroom1 n4</t>
+  </si>
+  <si>
+    <t>esd</t>
+  </si>
+  <si>
+    <t>6p molex</t>
+  </si>
+  <si>
+    <t>3p molex</t>
+  </si>
+  <si>
+    <t>100nF, 16V</t>
+  </si>
+  <si>
+    <t>3v3 5A</t>
+  </si>
+  <si>
+    <t>LM1084</t>
+  </si>
+  <si>
+    <t>10uF??? Tantal</t>
+  </si>
+  <si>
+    <t>10uF ceramic</t>
+  </si>
+  <si>
+    <t>22nF 50V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1uF tantal</t>
+  </si>
+  <si>
+    <t>&gt;30</t>
+  </si>
+  <si>
+    <t>&gt;80</t>
+  </si>
+  <si>
+    <t>10uF tantal 16V</t>
+  </si>
+  <si>
+    <t>4p molex</t>
+  </si>
+  <si>
+    <t>4p molex horiz</t>
   </si>
 </sst>
 </file>
@@ -593,7 +536,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,12 +730,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -800,12 +737,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,12 +929,9 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1011,25 +939,19 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
@@ -1041,9 +963,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1051,10 +970,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1435,14 +1357,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="35.81640625" customWidth="1"/>
-    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="58.81640625" customWidth="1"/>
+    <col min="3" max="3" width="45.90625" customWidth="1"/>
     <col min="4" max="4" width="57.08984375" customWidth="1"/>
     <col min="5" max="5" width="55" customWidth="1"/>
     <col min="6" max="6" width="35.6328125" customWidth="1"/>
@@ -1453,990 +1376,830 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>3</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="1">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="13"/>
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="G2" s="1"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="1">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="1">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1">
-        <v>4</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="1">
-        <v>20</v>
-      </c>
-      <c r="H6" s="1">
-        <v>5</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="1">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
-      <c r="I8" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="G8" s="1"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="1">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H9" s="1">
-        <v>8</v>
-      </c>
+      <c r="D9" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="1">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H10" s="1">
-        <v>9</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="G11" s="21">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="G11" s="1"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G12" s="1">
-        <v>10</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="1">
-        <v>6</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1">
-        <v>1</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="1">
-        <v>4</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="1">
-        <v>4</v>
-      </c>
-      <c r="H18" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="1">
-        <v>4</v>
-      </c>
-      <c r="H19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="1">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="1">
-        <v>7</v>
-      </c>
-      <c r="H20" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="1">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" s="20">
-        <v>3</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="20">
-        <v>3</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" s="1">
-        <v>8</v>
-      </c>
-      <c r="H24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="1">
-        <v>3</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="G27" s="1">
-        <v>5</v>
-      </c>
-      <c r="H27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="1">
         <v>2</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="1">
-        <v>5</v>
-      </c>
-      <c r="H28" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="1">
-        <v>3</v>
-      </c>
-      <c r="D29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="16">
         <v>6</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" s="1">
-        <v>12</v>
-      </c>
-      <c r="H29" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>81</v>
-      </c>
+      <c r="B30" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="16"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="1">
-        <v>5</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="1">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H32" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="C33" s="1">
-        <v>2</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35">
-        <f>SUM(C2:C34)</f>
-        <v>71</v>
-      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="B37" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1">
+        <v>9</v>
+      </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="E38" s="16">
+        <v>3</v>
+      </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B39" s="1"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B39" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1">
+        <v>6</v>
+      </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B40" s="1"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B40" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1">
+        <v>2</v>
+      </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B42" s="1"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B41" s="1">
+        <v>805</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B42" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C42" t="s">
+        <v>29</v>
+      </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="E42" s="1">
+        <v>7</v>
+      </c>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1">
+        <v>5</v>
+      </c>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B44" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1">
+        <v>4</v>
+      </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B45" s="1"/>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
       <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="E45" s="1">
+        <v>10</v>
+      </c>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B46" s="1"/>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B48" s="1"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B47" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B48" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="C48" s="1"/>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B50" s="1"/>
+      <c r="B50" s="1">
+        <v>805</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="B51" s="1">
+        <v>805</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="B52" s="1">
+        <v>805</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="E52" s="1">
+        <v>10</v>
+      </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B54" s="1"/>
+      <c r="B54" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B55" s="1"/>
+      <c r="B55" s="1">
+        <v>805</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
+      <c r="B56" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="E56" s="1">
+        <v>6</v>
+      </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="B57" s="1">
+        <v>805</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="E57" s="1">
+        <v>15</v>
+      </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B58" s="1"/>
+      <c r="B58" s="1">
+        <v>1206</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B59" s="1"/>
+      <c r="B59" s="1">
+        <v>805</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B61" s="1"/>
+      <c r="B61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B63" s="1"/>
@@ -2475,34 +2238,34 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F32" r:id="rId1" display="QRE1113 THT" xr:uid="{C7467625-A286-468E-8A7E-1A7A39BDECC1}"/>
-    <hyperlink ref="F3" r:id="rId2" display="0R" xr:uid="{C862754A-C382-43E8-A616-D2AF26643802}"/>
-    <hyperlink ref="F4" r:id="rId3" display="15R mouser" xr:uid="{DD575FCC-1415-4330-899B-C70DFF886B11}"/>
-    <hyperlink ref="F6" r:id="rId4" display="100R" xr:uid="{763E5EBB-5DD3-4781-B6D2-9F4C3D8344CC}"/>
-    <hyperlink ref="F5" r:id="rId5" display="10k mouser" xr:uid="{ED2B128C-C1AD-425C-8DC4-6214F339E204}"/>
-    <hyperlink ref="F30" r:id="rId6" xr:uid="{B596FF9F-B13C-40B2-A278-6278DE88A519}"/>
-    <hyperlink ref="F27" r:id="rId7" xr:uid="{3DE8E763-2485-4DF4-BCB1-A8CE5F2EC419}"/>
-    <hyperlink ref="F28" r:id="rId8" xr:uid="{019436FF-040E-4EB9-8335-60DF69292558}"/>
-    <hyperlink ref="F26" r:id="rId9" display="TSOP382. 38kHz" xr:uid="{37A8138D-E3CB-4172-AF64-8D059EB192A7}"/>
-    <hyperlink ref="F22" r:id="rId10" xr:uid="{7A7B8AF4-09CC-41E8-BA13-0E8B4DAA1724}"/>
-    <hyperlink ref="F23" r:id="rId11" xr:uid="{D071CBD8-5018-4961-9B17-F0BA82B3C326}"/>
-    <hyperlink ref="F21" r:id="rId12" display="USB C" xr:uid="{9DCBE1AD-73C2-4CF2-92FF-FAE0BDDC5F23}"/>
-    <hyperlink ref="F19" r:id="rId13" xr:uid="{132DDC0D-5C0A-439E-A3C6-C482F808FDEF}"/>
-    <hyperlink ref="F20" r:id="rId14" xr:uid="{FFF45319-FF1B-4F72-A21B-36978B113C9B}"/>
-    <hyperlink ref="F18" r:id="rId15" xr:uid="{AD263F34-F035-44E6-BCED-3EBC8E55851A}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{98A91549-44BB-43DE-82FA-759E9467366D}"/>
-    <hyperlink ref="F14" r:id="rId17" xr:uid="{7D16F510-0609-4A66-8417-B59F678FC2DE}"/>
-    <hyperlink ref="F10" r:id="rId18" xr:uid="{371B25F1-527B-4E70-B1F2-2BE6606DACEC}"/>
-    <hyperlink ref="F9" r:id="rId19" xr:uid="{929D84F0-E88E-4810-B009-80FE3FED9A37}"/>
-    <hyperlink ref="F29" r:id="rId20" xr:uid="{F6DBEFD4-801F-4613-95B3-A24ABBB0EBF1}"/>
-    <hyperlink ref="F25" r:id="rId21" display="ESP32 S3 WROOM1" xr:uid="{C2CDD0EF-FB14-4038-9794-A39B66094845}"/>
-    <hyperlink ref="F24" r:id="rId22" display="ESD protekce" xr:uid="{FB3BE120-E60B-4E64-87B8-658CEE0AACB7}"/>
-    <hyperlink ref="F8" r:id="rId23" display="22nF, 50V, 0805, mouser, X7R" xr:uid="{EF920451-0FF1-4E22-859F-6B07FF0D02EB}"/>
-    <hyperlink ref="F11" r:id="rId24" xr:uid="{5E8D4022-209B-4A78-A839-B160D615305B}"/>
-    <hyperlink ref="F12" r:id="rId25" xr:uid="{1DB20B2F-C9D6-4E69-A2DD-D42E31B3A79C}"/>
-    <hyperlink ref="F13" r:id="rId26" xr:uid="{5954B20F-A14D-45B1-9EAC-29E97102D58C}"/>
-    <hyperlink ref="F2" r:id="rId27" xr:uid="{F272AEEB-1F6E-41CC-B9EE-A0FD0E5C470F}"/>
-    <hyperlink ref="F33" r:id="rId28" xr:uid="{6ABF2726-A5C3-4787-BAF7-20B3D754FCE4}"/>
+    <hyperlink ref="D32" r:id="rId1" display="QRE1113 THT" xr:uid="{C7467625-A286-468E-8A7E-1A7A39BDECC1}"/>
+    <hyperlink ref="D3" r:id="rId2" display="0R" xr:uid="{C862754A-C382-43E8-A616-D2AF26643802}"/>
+    <hyperlink ref="D4" r:id="rId3" display="15R mouser" xr:uid="{DD575FCC-1415-4330-899B-C70DFF886B11}"/>
+    <hyperlink ref="D6" r:id="rId4" display="100R" xr:uid="{763E5EBB-5DD3-4781-B6D2-9F4C3D8344CC}"/>
+    <hyperlink ref="D5" r:id="rId5" display="10k mouser" xr:uid="{ED2B128C-C1AD-425C-8DC4-6214F339E204}"/>
+    <hyperlink ref="D30" r:id="rId6" xr:uid="{B596FF9F-B13C-40B2-A278-6278DE88A519}"/>
+    <hyperlink ref="D27" r:id="rId7" xr:uid="{3DE8E763-2485-4DF4-BCB1-A8CE5F2EC419}"/>
+    <hyperlink ref="D28" r:id="rId8" xr:uid="{019436FF-040E-4EB9-8335-60DF69292558}"/>
+    <hyperlink ref="D26" r:id="rId9" display="TSOP382. 38kHz" xr:uid="{37A8138D-E3CB-4172-AF64-8D059EB192A7}"/>
+    <hyperlink ref="D22" r:id="rId10" xr:uid="{7A7B8AF4-09CC-41E8-BA13-0E8B4DAA1724}"/>
+    <hyperlink ref="D23" r:id="rId11" xr:uid="{D071CBD8-5018-4961-9B17-F0BA82B3C326}"/>
+    <hyperlink ref="D21" r:id="rId12" display="USB C" xr:uid="{9DCBE1AD-73C2-4CF2-92FF-FAE0BDDC5F23}"/>
+    <hyperlink ref="D19" r:id="rId13" xr:uid="{132DDC0D-5C0A-439E-A3C6-C482F808FDEF}"/>
+    <hyperlink ref="D20" r:id="rId14" xr:uid="{FFF45319-FF1B-4F72-A21B-36978B113C9B}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{AD263F34-F035-44E6-BCED-3EBC8E55851A}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{98A91549-44BB-43DE-82FA-759E9467366D}"/>
+    <hyperlink ref="D14" r:id="rId17" xr:uid="{7D16F510-0609-4A66-8417-B59F678FC2DE}"/>
+    <hyperlink ref="D10" r:id="rId18" xr:uid="{371B25F1-527B-4E70-B1F2-2BE6606DACEC}"/>
+    <hyperlink ref="D9" r:id="rId19" xr:uid="{929D84F0-E88E-4810-B009-80FE3FED9A37}"/>
+    <hyperlink ref="D29" r:id="rId20" xr:uid="{F6DBEFD4-801F-4613-95B3-A24ABBB0EBF1}"/>
+    <hyperlink ref="D25" r:id="rId21" display="ESP32 S3 WROOM1" xr:uid="{C2CDD0EF-FB14-4038-9794-A39B66094845}"/>
+    <hyperlink ref="D24" r:id="rId22" display="ESD protekce" xr:uid="{FB3BE120-E60B-4E64-87B8-658CEE0AACB7}"/>
+    <hyperlink ref="D8" r:id="rId23" display="22nF, 50V, 0805, mouser, X7R" xr:uid="{EF920451-0FF1-4E22-859F-6B07FF0D02EB}"/>
+    <hyperlink ref="D11" r:id="rId24" xr:uid="{5E8D4022-209B-4A78-A839-B160D615305B}"/>
+    <hyperlink ref="D12" r:id="rId25" xr:uid="{1DB20B2F-C9D6-4E69-A2DD-D42E31B3A79C}"/>
+    <hyperlink ref="D13" r:id="rId26" xr:uid="{5954B20F-A14D-45B1-9EAC-29E97102D58C}"/>
+    <hyperlink ref="D2" r:id="rId27" xr:uid="{F272AEEB-1F6E-41CC-B9EE-A0FD0E5C470F}"/>
+    <hyperlink ref="D33" r:id="rId28" xr:uid="{6ABF2726-A5C3-4787-BAF7-20B3D754FCE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>

</xml_diff>

<commit_message>
BOM updates. mouser BOM added
</commit_message>
<xml_diff>
--- a/- DOCS -/COMPONENTS LIST/After_Rybnik_BOM.xlsx
+++ b/- DOCS -/COMPONENTS LIST/After_Rybnik_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\RoboCop\- DOCS -\COMPONENTS LIST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80479926-2EB1-409A-9BF6-7857101E683B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367403A2-75A3-4689-9A88-66E9FBE93256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD 1206" sheetId="2" r:id="rId1"/>
@@ -1276,17 +1276,17 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D11" sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
-    <col min="3" max="3" width="39.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1206</v>
       </c>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1206</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1206</v>
       </c>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1206</v>
       </c>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1206</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1206</v>
       </c>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1206</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1206</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1206</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1206</v>
       </c>
@@ -1441,19 +1441,19 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E10"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>805</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>805</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>805</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>805</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>805</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>805</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>805</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>805</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>805</v>
       </c>
@@ -1587,10 +1587,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
     </row>
   </sheetData>
@@ -1613,25 +1613,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.81640625" customWidth="1"/>
-    <col min="2" max="2" width="31.36328125" customWidth="1"/>
-    <col min="3" max="3" width="45.90625" customWidth="1"/>
-    <col min="4" max="4" width="57.08984375" customWidth="1"/>
+    <col min="1" max="1" width="53.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" customWidth="1"/>
     <col min="5" max="5" width="55" customWidth="1"/>
-    <col min="6" max="6" width="35.6328125" customWidth="1"/>
-    <col min="7" max="7" width="23.90625" customWidth="1"/>
-    <col min="8" max="8" width="7.26953125" customWidth="1"/>
-    <col min="9" max="9" width="34.54296875" customWidth="1"/>
-    <col min="10" max="10" width="36.81640625" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="G2" s="1"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
@@ -1747,7 +1747,7 @@
       <c r="G8" s="1"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1792,7 +1792,7 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -1888,12 +1888,12 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1901,7 +1901,7 @@
       <c r="F20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1909,129 +1909,129 @@
       <c r="F21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="D32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="D36" s="1"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="D37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F46" s="1"/>
     </row>
-    <row r="49" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F52" s="1"/>
     </row>
-    <row r="54" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>

</xml_diff>